<commit_message>
3 final projects + micro section readings
</commit_message>
<xml_diff>
--- a/Rmd-Repo/current grade calcs.xlsx
+++ b/Rmd-Repo/current grade calcs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arunk\Documents\GitHub\arun-krishnaraj.github.io\Rmd-Repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arunk/Documents/GitHub/arun-krishnaraj.github.io/Rmd-Repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E15AB430-2582-41F8-9BF4-66E9D85D8E3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AE2A8F-5FEE-2048-8D9B-1520E2C06D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20E5DBA4-6F28-4B38-8EB4-07C7B84E68CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{20E5DBA4-6F28-4B38-8EB4-07C7B84E68CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -213,9 +212,6 @@
     <t>graded?</t>
   </si>
   <si>
-    <t>SDS328M</t>
-  </si>
-  <si>
     <t>Grade (pts)</t>
   </si>
   <si>
@@ -310,6 +306,9 @@
   </si>
   <si>
     <t>all projects must be submitted to pass</t>
+  </si>
+  <si>
+    <t>SDS348</t>
   </si>
 </sst>
 </file>
@@ -318,7 +317,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000000000000%"/>
-    <numFmt numFmtId="166" formatCode="0.00000000000000%"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -444,6 +443,20 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -453,20 +466,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,77 +783,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DCF9B3-ACF7-4F83-BAB5-BD78879A182E}">
   <dimension ref="A1:AF44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z20" sqref="Z20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" customWidth="1"/>
-    <col min="26" max="26" width="10.7109375" customWidth="1"/>
+    <col min="26" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="6" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="14"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="11"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -868,8 +867,8 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="6" t="s">
         <v>39</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -891,44 +890,44 @@
         <v>58</v>
       </c>
       <c r="O2" s="1"/>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="19" t="s">
+      <c r="Q2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="R2" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="S2" s="19"/>
+      <c r="S2" s="16"/>
       <c r="T2" s="1"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="9" t="s">
+      <c r="U2" s="7"/>
+      <c r="V2" s="6" t="s">
         <v>39</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z2" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AA2" s="13" t="s">
-        <v>83</v>
+      <c r="Z2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
-      <c r="AF2" s="10"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="AF2" s="7"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
@@ -944,8 +943,8 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="9" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="6" t="s">
         <v>40</v>
       </c>
       <c r="I3" s="1">
@@ -963,7 +962,7 @@
         <f>LARGE($K$3:$K$10,1)</f>
         <v>1.0666666666666667</v>
       </c>
-      <c r="M3" s="15">
+      <c r="M3" s="12">
         <v>0.08</v>
       </c>
       <c r="N3" s="1">
@@ -973,8 +972,8 @@
       <c r="O3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="9" t="s">
-        <v>62</v>
+      <c r="P3" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="Q3" s="1">
         <v>20</v>
@@ -985,15 +984,15 @@
       </c>
       <c r="S3" s="1">
         <f>SUM(Q3:Q14)-SUM(SMALL(Q3:Q14,1))</f>
-        <v>98.5</v>
+        <v>118.5</v>
       </c>
       <c r="T3" s="1">
         <f>SUM(R3:R14)-SUM(SMALL(R3:R14,1))</f>
-        <v>100</v>
-      </c>
-      <c r="U3" s="10"/>
-      <c r="V3" s="9" t="s">
-        <v>62</v>
+        <v>120</v>
+      </c>
+      <c r="U3" s="7"/>
+      <c r="V3" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="W3" s="1">
         <v>100</v>
@@ -1005,20 +1004,20 @@
         <f>(SUM(W3:W10)-SMALL(W3:W10,1))/700</f>
         <v>0.99571428571428566</v>
       </c>
-      <c r="Z3" s="22">
+      <c r="Z3" s="19">
         <v>0.7</v>
       </c>
-      <c r="AA3" s="9"/>
+      <c r="AA3" s="6"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="10"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="AF3" s="7"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
@@ -1033,8 +1032,8 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="9" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="1">
@@ -1055,7 +1054,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q4" s="1">
@@ -1067,8 +1066,8 @@
       </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="9" t="s">
+      <c r="U4" s="7"/>
+      <c r="V4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="W4" s="1">
@@ -1078,9 +1077,9 @@
         <v>100</v>
       </c>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="9" t="s">
-        <v>84</v>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="AB4" s="1">
         <v>79</v>
@@ -1093,15 +1092,15 @@
       </c>
       <c r="AE4" s="1">
         <f>AVERAGE(AB4:AB6)</f>
-        <v>89</v>
-      </c>
-      <c r="AF4" s="10">
+        <v>89.666666666666671</v>
+      </c>
+      <c r="AF4" s="7">
         <f>AVERAGE(AD4:AD6)</f>
-        <v>82.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+        <v>83.033333333333346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1"/>
@@ -1115,8 +1114,8 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="9" t="s">
+      <c r="G5" s="7"/>
+      <c r="H5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="1">
@@ -1137,7 +1136,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="Q5" s="1">
@@ -1149,8 +1148,8 @@
       </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="9" t="s">
+      <c r="U5" s="7"/>
+      <c r="V5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="W5" s="1">
@@ -1160,9 +1159,9 @@
         <v>100</v>
       </c>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="9" t="s">
-        <v>85</v>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="AB5" s="1">
         <v>99</v>
@@ -1174,10 +1173,10 @@
         <v>86.5</v>
       </c>
       <c r="AE5" s="1"/>
-      <c r="AF5" s="10"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="AF5" s="7"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1"/>
@@ -1191,8 +1190,8 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="9" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="1">
@@ -1213,7 +1212,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="9" t="s">
+      <c r="P6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="Q6" s="1">
@@ -1225,8 +1224,8 @@
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="9" t="s">
+      <c r="U6" s="7"/>
+      <c r="V6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="W6" s="1">
@@ -1236,20 +1235,24 @@
         <v>100</v>
       </c>
       <c r="Y6" s="1"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB6" s="1"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>91</v>
+      </c>
       <c r="AC6" s="1">
         <v>100</v>
       </c>
-      <c r="AD6" s="1"/>
+      <c r="AD6" s="1">
+        <v>83.7</v>
+      </c>
       <c r="AE6" s="1"/>
-      <c r="AF6" s="10"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="AF6" s="7"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1">
@@ -1270,8 +1273,8 @@
         <f>SUM(D7:D14)</f>
         <v>21</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="9" t="s">
+      <c r="G7" s="7"/>
+      <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I7" s="1">
@@ -1292,7 +1295,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="9" t="s">
+      <c r="P7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="Q7" s="1">
@@ -1304,8 +1307,8 @@
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="9" t="s">
+      <c r="U7" s="7"/>
+      <c r="V7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="W7" s="1">
@@ -1315,16 +1318,16 @@
         <v>100</v>
       </c>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="10"/>
-      <c r="AA7" s="9"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="6"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
-      <c r="AF7" s="10"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="AF7" s="7"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1">
@@ -1343,8 +1346,8 @@
         <f>SUM(C7:C16)</f>
         <v>21</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="9" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="1">
@@ -1365,7 +1368,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="9" t="s">
+      <c r="P8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="Q8" s="1">
@@ -1377,8 +1380,8 @@
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="9" t="s">
+      <c r="U8" s="7"/>
+      <c r="V8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="W8" s="1">
@@ -1388,18 +1391,18 @@
         <v>100</v>
       </c>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="9" t="s">
-        <v>87</v>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
-      <c r="AF8" s="10"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="AF8" s="7"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1">
@@ -1415,8 +1418,8 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="9" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="1">
@@ -1432,23 +1435,25 @@
       </c>
       <c r="L9" s="3">
         <f>LARGE($K$3:$K$10,7)</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="9" t="s">
+      <c r="P9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1" t="str">
+      <c r="Q9" s="16">
+        <v>20</v>
+      </c>
+      <c r="R9" s="1">
         <f t="shared" si="3"/>
-        <v/>
+        <v>20</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="9" t="s">
+      <c r="U9" s="7"/>
+      <c r="V9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="W9" s="1">
@@ -1458,18 +1463,18 @@
         <v>100</v>
       </c>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="10"/>
-      <c r="AA9" s="11" t="s">
-        <v>89</v>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="AB9" s="4"/>
       <c r="AC9" s="4"/>
       <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
-      <c r="AF9" s="12"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="AF9" s="9"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1">
@@ -1485,27 +1490,32 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="9" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1" t="str">
+      <c r="I10" s="16">
+        <v>12</v>
+      </c>
+      <c r="J10" s="1">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K10" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="K10" s="3">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L10" s="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="L10" s="3">
+        <f>LARGE($K$3:$K$10,8)</f>
+        <v>0.6</v>
+      </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="1" t="str">
+      <c r="N10" s="1">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="O10" s="1"/>
-      <c r="P10" s="9" t="s">
+      <c r="P10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Q10" s="1"/>
@@ -1515,8 +1525,8 @@
       </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="9" t="s">
+      <c r="U10" s="7"/>
+      <c r="V10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="W10" s="1">
@@ -1526,10 +1536,10 @@
         <v>100</v>
       </c>
       <c r="Y10" s="1"/>
-      <c r="Z10" s="10"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="Z10" s="7"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="1">
@@ -1545,8 +1555,8 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="13" t="s">
+      <c r="G11" s="7"/>
+      <c r="H11" s="10" t="s">
         <v>50</v>
       </c>
       <c r="I11" s="1">
@@ -1563,7 +1573,7 @@
         <f>LARGE($K$11:$K$20,1)</f>
         <v>1</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="12">
         <v>0.08</v>
       </c>
       <c r="N11" s="1">
@@ -1573,7 +1583,7 @@
       <c r="O11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="13" t="s">
+      <c r="P11" s="10" t="s">
         <v>19</v>
       </c>
       <c r="Q11" s="1"/>
@@ -1583,21 +1593,21 @@
       </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="13" t="s">
-        <v>76</v>
+      <c r="U11" s="7"/>
+      <c r="V11" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="W11" s="1"/>
       <c r="X11" s="1">
         <v>100</v>
       </c>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="22">
+      <c r="Z11" s="19">
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="1">
@@ -1613,8 +1623,8 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="13" t="s">
+      <c r="G12" s="7"/>
+      <c r="H12" s="10" t="s">
         <v>51</v>
       </c>
       <c r="I12" s="1">
@@ -1634,7 +1644,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="13" t="s">
+      <c r="P12" s="10" t="s">
         <v>22</v>
       </c>
       <c r="Q12" s="1"/>
@@ -1644,19 +1654,19 @@
       </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="13" t="s">
-        <v>77</v>
+      <c r="U12" s="7"/>
+      <c r="V12" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="W12" s="1"/>
       <c r="X12" s="1">
         <v>80</v>
       </c>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="10"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="Z12" s="7"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="1">
@@ -1672,8 +1682,8 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="13" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="10" t="s">
         <v>52</v>
       </c>
       <c r="I13" s="1">
@@ -1693,7 +1703,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="13" t="s">
+      <c r="P13" s="10" t="s">
         <v>21</v>
       </c>
       <c r="Q13" s="1"/>
@@ -1703,22 +1713,22 @@
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="13" t="s">
-        <v>78</v>
+      <c r="U13" s="7"/>
+      <c r="V13" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="W13" s="1"/>
       <c r="X13" s="1">
         <v>20</v>
       </c>
       <c r="Y13" s="1"/>
-      <c r="Z13" s="10"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="Z13" s="7"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -1729,8 +1739,8 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="9" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I14" s="1">
@@ -1750,7 +1760,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="13" t="s">
+      <c r="P14" s="10" t="s">
         <v>23</v>
       </c>
       <c r="Q14" s="1"/>
@@ -1760,22 +1770,22 @@
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="13" t="s">
-        <v>79</v>
+      <c r="U14" s="7"/>
+      <c r="V14" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="22">
+      <c r="Z14" s="19">
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -1786,8 +1796,8 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="9" t="s">
+      <c r="G15" s="7"/>
+      <c r="H15" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I15" s="1">
@@ -1807,8 +1817,8 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="13" t="s">
-        <v>63</v>
+      <c r="P15" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="Q15" s="1">
         <v>10</v>
@@ -1819,24 +1829,24 @@
       </c>
       <c r="S15" s="1">
         <f>SUM(Q15:Q27)-SUM(SMALL(Q15:Q27,1))</f>
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="T15" s="1">
         <f>SUM(R15:R27)-SUM(SMALL(R15:R27,1))</f>
-        <v>90</v>
-      </c>
-      <c r="U15" s="10"/>
-      <c r="V15" s="9"/>
+        <v>110</v>
+      </c>
+      <c r="U15" s="7"/>
+      <c r="V15" s="6"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
-      <c r="Z15" s="10"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="Z15" s="7"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -1847,8 +1857,8 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="9" t="s">
+      <c r="G16" s="7"/>
+      <c r="H16" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I16" s="1">
@@ -1863,12 +1873,12 @@
       </c>
       <c r="L16" s="3">
         <f>LARGE($K$11:$K$20,6)</f>
-        <v>0.83333333333333337</v>
+        <v>0.92</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="9" t="s">
+      <c r="P16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q16" s="1">
@@ -1880,27 +1890,27 @@
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="9"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="6"/>
       <c r="W16" s="1"/>
       <c r="X16" s="3">
         <f>SUMPRODUCT(Y3:Y14,Z3:Z14)</f>
         <v>0.69699999999999995</v>
       </c>
       <c r="Y16" s="1"/>
-      <c r="Z16" s="10"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="Z16" s="7"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="9" t="s">
+      <c r="G17" s="7"/>
+      <c r="H17" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I17" s="1">
@@ -1915,12 +1925,12 @@
       </c>
       <c r="L17" s="3">
         <f>LARGE($K$11:$K$20,7)</f>
-        <v>0.75</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="9" t="s">
+      <c r="P17" s="6" t="s">
         <v>13</v>
       </c>
       <c r="Q17" s="1">
@@ -1932,17 +1942,17 @@
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="9"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="6"/>
       <c r="W17" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
-      <c r="Z17" s="10"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="Z17" s="7"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="1"/>
@@ -1950,24 +1960,31 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="9" t="s">
+      <c r="G18" s="7"/>
+      <c r="H18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="3" t="str">
+      <c r="I18" s="16">
+        <v>46</v>
+      </c>
+      <c r="J18" s="16">
+        <v>50</v>
+      </c>
+      <c r="K18" s="3">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L18" s="3"/>
+        <v>0.92</v>
+      </c>
+      <c r="L18" s="3">
+        <f>LARGE($K$11:$K$20,8)</f>
+        <v>0.75</v>
+      </c>
       <c r="M18" s="1"/>
-      <c r="N18" s="1" t="str">
+      <c r="N18" s="1">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="O18" s="1"/>
-      <c r="P18" s="9" t="s">
+      <c r="P18" s="6" t="s">
         <v>14</v>
       </c>
       <c r="Q18" s="1">
@@ -1979,17 +1996,17 @@
       </c>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
-      <c r="U18" s="10"/>
+      <c r="U18" s="7"/>
       <c r="V18" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
-      <c r="Z18" s="12"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="Z18" s="9"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="1">
@@ -2010,8 +2027,8 @@
         <f>SUM(D19:D26)</f>
         <v>33.5</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="9" t="s">
+      <c r="G19" s="7"/>
+      <c r="H19" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="1"/>
@@ -2027,7 +2044,7 @@
         <v/>
       </c>
       <c r="O19" s="1"/>
-      <c r="P19" s="9" t="s">
+      <c r="P19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="Q19" s="1">
@@ -2039,10 +2056,10 @@
       </c>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
-      <c r="U19" s="10"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="U19" s="7"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1">
@@ -2061,8 +2078,8 @@
         <f>SUM(C19:C26)</f>
         <v>35</v>
       </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="9" t="s">
+      <c r="G20" s="7"/>
+      <c r="H20" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I20" s="1"/>
@@ -2078,7 +2095,7 @@
         <v/>
       </c>
       <c r="O20" s="1"/>
-      <c r="P20" s="9" t="s">
+      <c r="P20" s="6" t="s">
         <v>16</v>
       </c>
       <c r="Q20" s="1">
@@ -2090,10 +2107,10 @@
       </c>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
-      <c r="U20" s="10"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="U20" s="7"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="1">
@@ -2109,8 +2126,8 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="13" t="s">
+      <c r="G21" s="7"/>
+      <c r="H21" s="10" t="s">
         <v>42</v>
       </c>
       <c r="I21" s="1">
@@ -2124,15 +2141,15 @@
         <v>0.95</v>
       </c>
       <c r="L21" s="3"/>
-      <c r="M21" s="15">
+      <c r="M21" s="12">
         <v>0.12</v>
       </c>
       <c r="N21" s="1">
-        <f>IF(I21="","",1)</f>
+        <f t="shared" ref="N21:N27" si="9">IF(I21="","",1)</f>
         <v>1</v>
       </c>
       <c r="O21" s="1"/>
-      <c r="P21" s="9" t="s">
+      <c r="P21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="Q21" s="1">
@@ -2144,10 +2161,10 @@
       </c>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
-      <c r="U21" s="10"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="U21" s="7"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="1">
@@ -2163,8 +2180,8 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="13" t="s">
+      <c r="G22" s="7"/>
+      <c r="H22" s="10" t="s">
         <v>43</v>
       </c>
       <c r="I22" s="1">
@@ -2178,15 +2195,15 @@
         <v>1</v>
       </c>
       <c r="L22" s="3"/>
-      <c r="M22" s="15">
+      <c r="M22" s="12">
         <v>0.12</v>
       </c>
       <c r="N22" s="1">
-        <f>IF(I22="","",1)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O22" s="1"/>
-      <c r="P22" s="9" t="s">
+      <c r="P22" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Q22" s="1">
@@ -2198,10 +2215,10 @@
       </c>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
-      <c r="U22" s="10"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="U22" s="7"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="1">
@@ -2217,8 +2234,8 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="13" t="s">
+      <c r="G23" s="7"/>
+      <c r="H23" s="10" t="s">
         <v>44</v>
       </c>
       <c r="I23" s="1"/>
@@ -2228,15 +2245,15 @@
         <v/>
       </c>
       <c r="L23" s="3"/>
-      <c r="M23" s="15">
+      <c r="M23" s="12">
         <v>0.12</v>
       </c>
       <c r="N23" s="1" t="str">
-        <f>IF(I23="","",1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O23" s="1"/>
-      <c r="P23" s="13" t="s">
+      <c r="P23" s="10" t="s">
         <v>19</v>
       </c>
       <c r="Q23" s="1">
@@ -2248,10 +2265,10 @@
       </c>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
-      <c r="U23" s="10"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="U23" s="7"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="1">
@@ -2267,8 +2284,8 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="13" t="s">
+      <c r="G24" s="7"/>
+      <c r="H24" s="10" t="s">
         <v>45</v>
       </c>
       <c r="I24" s="1"/>
@@ -2278,15 +2295,15 @@
         <v/>
       </c>
       <c r="L24" s="3"/>
-      <c r="M24" s="15">
+      <c r="M24" s="12">
         <v>0.12</v>
       </c>
       <c r="N24" s="1" t="str">
-        <f>IF(I24="","",1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O24" s="1"/>
-      <c r="P24" s="13" t="s">
+      <c r="P24" s="10" t="s">
         <v>22</v>
       </c>
       <c r="Q24" s="1">
@@ -2298,10 +2315,10 @@
       </c>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
-      <c r="U24" s="10"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="U24" s="7"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="1">
@@ -2317,8 +2334,8 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="13" t="s">
+      <c r="G25" s="7"/>
+      <c r="H25" s="10" t="s">
         <v>46</v>
       </c>
       <c r="I25" s="1">
@@ -2332,30 +2349,32 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="L25" s="3"/>
-      <c r="M25" s="15">
+      <c r="M25" s="12">
         <v>0.12</v>
       </c>
       <c r="N25" s="1">
-        <f>IF(I25="","",1)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P25" s="13" t="s">
+      <c r="P25" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1" t="str">
+      <c r="Q25" s="16">
+        <v>10</v>
+      </c>
+      <c r="R25" s="1">
         <f t="shared" si="7"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
-      <c r="U25" s="10"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="U25" s="7"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="1"/>
@@ -2369,8 +2388,8 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="13" t="s">
+      <c r="G26" s="7"/>
+      <c r="H26" s="10" t="s">
         <v>43</v>
       </c>
       <c r="I26" s="1">
@@ -2384,28 +2403,30 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="L26" s="3"/>
-      <c r="M26" s="15">
+      <c r="M26" s="12">
         <v>0.12</v>
       </c>
       <c r="N26" s="1">
-        <f>IF(I26="","",1)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O26" s="1"/>
-      <c r="P26" s="13" t="s">
+      <c r="P26" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1" t="str">
+      <c r="Q26" s="16">
+        <v>10</v>
+      </c>
+      <c r="R26" s="1">
         <f t="shared" si="7"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
-      <c r="U26" s="10"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="U26" s="7"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="1"/>
@@ -2413,8 +2434,8 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="13" t="s">
+      <c r="G27" s="7"/>
+      <c r="H27" s="10" t="s">
         <v>44</v>
       </c>
       <c r="I27" s="1"/>
@@ -2424,16 +2445,16 @@
         <v/>
       </c>
       <c r="L27" s="3"/>
-      <c r="M27" s="15">
+      <c r="M27" s="12">
         <v>0.12</v>
       </c>
       <c r="N27" s="1" t="str">
-        <f>IF(I27="","",1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O27" s="1"/>
-      <c r="P27" s="13" t="s">
-        <v>64</v>
+      <c r="P27" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="Q27" s="1"/>
       <c r="R27" s="1" t="str">
@@ -2442,10 +2463,10 @@
       </c>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
-      <c r="U27" s="10"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="U27" s="7"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="1"/>
@@ -2456,8 +2477,8 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="9"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="6"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -2465,7 +2486,7 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="P28" s="13" t="s">
+      <c r="P28" s="10" t="s">
         <v>42</v>
       </c>
       <c r="Q28" s="1">
@@ -2477,10 +2498,10 @@
       </c>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
-      <c r="U28" s="10"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="U28" s="7"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="1">
@@ -2496,22 +2517,22 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="9"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="6"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="15" t="s">
+      <c r="M29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="N29" s="16">
-        <f>AVERAGE(L3:L7)*M3+AVERAGE(L11:L15)*M11+SUMPRODUCT(K21:K27,M21:M27)</f>
-        <v>0.6587466666666667</v>
+      <c r="N29" s="13">
+        <f>AVERAGE(L3:L8)*M3+AVERAGE(L11:L16)*M11+SUMPRODUCT(K21:K27,M21:M27)</f>
+        <v>0.65577777777777779</v>
       </c>
       <c r="O29" s="1"/>
-      <c r="P29" s="13" t="s">
-        <v>65</v>
+      <c r="P29" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="Q29" s="1"/>
       <c r="R29" s="1" t="str">
@@ -2520,10 +2541,10 @@
       </c>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
-      <c r="U29" s="10"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="U29" s="7"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="1">
@@ -2539,15 +2560,15 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="9"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="6"/>
       <c r="I30" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="17" t="s">
+      <c r="M30" s="14" t="s">
         <v>57</v>
       </c>
       <c r="N30" s="3">
@@ -2555,8 +2576,8 @@
         <v>0.64</v>
       </c>
       <c r="O30" s="1"/>
-      <c r="P30" s="13" t="s">
-        <v>66</v>
+      <c r="P30" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="Q30" s="1"/>
       <c r="R30" s="1" t="str">
@@ -2565,10 +2586,10 @@
       </c>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
-      <c r="U30" s="10"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="U30" s="7"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B31" s="1"/>
@@ -2582,10 +2603,10 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="9"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="6"/>
       <c r="I31" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -2593,28 +2614,28 @@
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="P31" s="13" t="s">
-        <v>67</v>
+      <c r="P31" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="Q31" s="1">
         <v>5</v>
       </c>
       <c r="R31" s="1">
-        <f>IF(Q31="","",5)</f>
+        <f t="shared" ref="R31:R36" si="10">IF(Q31="","",5)</f>
         <v>5</v>
       </c>
       <c r="S31" s="1">
         <f>SUM(Q31:Q36)-SUM(SMALL(Q31:Q36,1))</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="T31" s="1">
         <f>SUM(R31:R36)-SUM(SMALL(R31:R36,1))</f>
-        <v>20</v>
-      </c>
-      <c r="U31" s="10"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="U31" s="7"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="1"/>
@@ -2628,56 +2649,56 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="11"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="8"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
-      <c r="N32" s="18">
+      <c r="N32" s="15">
         <f>N29/N30</f>
-        <v>1.0292916666666667</v>
+        <v>1.0246527777777779</v>
       </c>
       <c r="O32" s="4"/>
-      <c r="P32" s="9" t="s">
+      <c r="P32" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q32" s="1">
         <v>5</v>
       </c>
       <c r="R32" s="1">
-        <f>IF(Q32="","",5)</f>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
-      <c r="U32" s="10"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
+      <c r="U32" s="7"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="10"/>
-      <c r="P33" s="9" t="s">
+      <c r="G33" s="7"/>
+      <c r="P33" s="6" t="s">
         <v>13</v>
       </c>
       <c r="Q33" s="1">
         <v>5</v>
       </c>
       <c r="R33" s="1">
-        <f>IF(Q33="","",5)</f>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
-      <c r="U33" s="10"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
+      <c r="U33" s="7"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A34" s="6"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1">
         <f>SUM(C3:C6,F8,F20,C29:C32)</f>
@@ -2689,23 +2710,23 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="10"/>
-      <c r="P34" s="9" t="s">
+      <c r="G34" s="7"/>
+      <c r="P34" s="6" t="s">
         <v>14</v>
       </c>
       <c r="Q34" s="1">
         <v>5</v>
       </c>
       <c r="R34" s="1">
-        <f>IF(Q34="","",5)</f>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
-      <c r="U34" s="10"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
+      <c r="U34" s="7"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" s="6"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1">
         <f>D34/C34</f>
@@ -2714,45 +2735,46 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="10"/>
-      <c r="P35" s="9" t="s">
+      <c r="G35" s="7"/>
+      <c r="P35" s="6" t="s">
         <v>15</v>
       </c>
       <c r="Q35" s="1">
         <v>5</v>
       </c>
       <c r="R35" s="1">
-        <f>IF(Q35="","",5)</f>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
-      <c r="U35" s="10"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
+      <c r="U35" s="7"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" s="6"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="10"/>
-      <c r="P36" s="9" t="s">
+      <c r="G36" s="7"/>
+      <c r="P36" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="1" t="str">
-        <f>IF(Q36="","",5)</f>
-        <v/>
+      <c r="Q36" s="16">
+        <v>5</v>
+      </c>
+      <c r="R36" s="1">
+        <v>5</v>
       </c>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
-      <c r="U36" s="10"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
+      <c r="U36" s="7"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
       <c r="B37" s="1" t="s">
         <v>27</v>
       </c>
@@ -2766,37 +2788,37 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="10"/>
-      <c r="P37" s="9"/>
+      <c r="G37" s="7"/>
+      <c r="P37" s="6"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
-      <c r="U37" s="10"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
+      <c r="U37" s="7"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A38" s="6"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="10"/>
-      <c r="P38" s="9"/>
+      <c r="G38" s="7"/>
+      <c r="P38" s="6"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1">
         <f>SUM(S3,S15,Q28,S31)</f>
-        <v>328.5</v>
+        <v>373.5</v>
       </c>
       <c r="T38" s="1">
         <f>SUM(T3,T15,R28,T31)</f>
-        <v>330</v>
-      </c>
-      <c r="U38" s="10"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
+        <v>375</v>
+      </c>
+      <c r="U38" s="7"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
       <c r="B39" s="1">
         <v>360</v>
       </c>
@@ -2812,26 +2834,26 @@
       <c r="F39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="G39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P39" s="9"/>
+      <c r="P39" s="6"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T39" s="1">
         <f>T38-S38</f>
         <v>1.5</v>
       </c>
-      <c r="U39" s="10" t="str">
+      <c r="U39" s="7" t="str">
         <f>IF(Q42&gt;T39,R42,IF(Q43&gt;T39,R43,IF(Q44&gt;T39,R44,"0")))</f>
         <v>A</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A40" s="6"/>
       <c r="B40" s="1" t="s">
         <v>28</v>
       </c>
@@ -2849,20 +2871,20 @@
       <c r="F40" s="3">
         <v>0.85</v>
       </c>
-      <c r="G40" s="10" t="s">
+      <c r="G40" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P40" s="9">
+      <c r="P40" s="6">
         <v>700</v>
       </c>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
-      <c r="U40" s="10"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
+      <c r="U40" s="7"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1">
         <f>D40-1</f>
@@ -2879,24 +2901,24 @@
       <c r="F41" s="3">
         <v>0.8</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G41" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="P41" s="9" t="s">
+      <c r="P41" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q41" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="R41" s="1" t="s">
         <v>29</v>
       </c>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
-      <c r="U41" s="10"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
+      <c r="U41" s="7"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A42" s="6"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1">
         <f>D41-1</f>
@@ -2913,10 +2935,10 @@
       <c r="F42" s="3">
         <v>0.75</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="G42" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="P42" s="9">
+      <c r="P42" s="6">
         <v>658</v>
       </c>
       <c r="Q42" s="1">
@@ -2928,10 +2950,10 @@
       </c>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
-      <c r="U42" s="10"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
+      <c r="U42" s="7"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A43" s="6"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1">
         <f>D42-1</f>
@@ -2948,10 +2970,10 @@
       <c r="F43" s="3">
         <v>0.7</v>
       </c>
-      <c r="G43" s="10" t="s">
+      <c r="G43" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="P43" s="9">
+      <c r="P43" s="6">
         <v>630</v>
       </c>
       <c r="Q43" s="1">
@@ -2959,14 +2981,14 @@
         <v>70</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
-      <c r="U43" s="10"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+      <c r="U43" s="7"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A44" s="8"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4">
         <f>D43-1</f>
@@ -2983,10 +3005,10 @@
       <c r="F44" s="5">
         <v>0.65</v>
       </c>
-      <c r="G44" s="12" t="s">
+      <c r="G44" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="P44" s="11">
+      <c r="P44" s="8">
         <v>609</v>
       </c>
       <c r="Q44" s="4">
@@ -2998,7 +3020,7 @@
       </c>
       <c r="S44" s="4"/>
       <c r="T44" s="4"/>
-      <c r="U44" s="12"/>
+      <c r="U44" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>